<commit_message>
Implementation of REGEX into GUI
</commit_message>
<xml_diff>
--- a/ATSbotDB.xlsx
+++ b/ATSbotDB.xlsx
@@ -392,7 +392,7 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>ESD320S620DT</t>
+          <t>EUD150S560DTA</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
-          <t>EUD150S350DTA</t>
+          <t>EUD150S560DTA</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added regex to validate
</commit_message>
<xml_diff>
--- a/ATSbotDB.xlsx
+++ b/ATSbotDB.xlsx
@@ -497,7 +497,7 @@
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>EUD150S560DTA</t>
+          <t>EUD150S350DTA</t>
         </is>
       </c>
     </row>
@@ -542,7 +542,7 @@
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>ESD240S660DT</t>
+          <t>EUD150S560DTA</t>
         </is>
       </c>
     </row>

</xml_diff>